<commit_message>
stabilised DB tables of properties_amenities and looks like it is working ok
</commit_message>
<xml_diff>
--- a/other_files/all_amenities.xlsx
+++ b/other_files/all_amenities.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>amenity</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>theatre</t>
+  </si>
+  <si>
+    <t>1=important</t>
+  </si>
+  <si>
+    <t>2=medium</t>
+  </si>
+  <si>
+    <t>3= less important</t>
   </si>
 </sst>
 </file>
@@ -1145,163 +1154,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A102"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1386,272 +1417,290 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>

</xml_diff>